<commit_message>
Add floating point adder and dependencies
</commit_message>
<xml_diff>
--- a/Reports/VLSI Project Reports.xlsx
+++ b/Reports/VLSI Project Reports.xlsx
@@ -766,7 +766,7 @@
         <v>17209.6</v>
       </c>
       <c r="N7" s="20">
-        <v>2314.8</v>
+        <v>28.81</v>
       </c>
       <c r="O7" s="20">
         <v>1290.4</v>
@@ -1189,15 +1189,23 @@
       </c>
       <c r="P17" s="18"/>
       <c r="Q17" s="20">
-        <v>2305.0</v>
-      </c>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="20"/>
+        <v>1144.0</v>
+      </c>
+      <c r="R17" s="20">
+        <v>3758.4</v>
+      </c>
+      <c r="S17" s="20">
+        <v>16700.4</v>
+      </c>
+      <c r="T17" s="20">
+        <v>14741.6</v>
+      </c>
       <c r="U17" s="20">
-        <v>1754.5</v>
-      </c>
-      <c r="V17" s="20"/>
+        <v>99.17</v>
+      </c>
+      <c r="V17" s="20">
+        <v>3758.4</v>
+      </c>
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
     </row>

</xml_diff>